<commit_message>
Fixed Excel template generator
</commit_message>
<xml_diff>
--- a/docs/Finance/templates/Ledger.xlsx
+++ b/docs/Finance/templates/Ledger.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
   <si>
     <t>ledger</t>
   </si>
@@ -28,51 +28,78 @@
     <t/>
   </si>
   <si>
+    <t>Ledger Id</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
     <t>varchar(4), PK, NN</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
     <t>varchar(100), NN</t>
   </si>
   <si>
+    <t>Leading ledger indicator</t>
+  </si>
+  <si>
     <t>leading</t>
   </si>
   <si>
     <t>boolean, NN</t>
   </si>
   <si>
+    <t>Ledger Type</t>
+  </si>
+  <si>
     <t>ledger_type</t>
   </si>
   <si>
     <t>ledger_type, NN</t>
   </si>
   <si>
+    <t>Underlying ledger</t>
+  </si>
+  <si>
     <t>underlying_ledger</t>
   </si>
   <si>
     <t>varchar(4)</t>
   </si>
   <si>
+    <t>User created record</t>
+  </si>
+  <si>
     <t>created_by</t>
   </si>
   <si>
     <t>varchar(20), NN</t>
   </si>
   <si>
+    <t>Timestamp of record create</t>
+  </si>
+  <si>
     <t>created_at</t>
   </si>
   <si>
     <t>timestamptz, NN</t>
   </si>
   <si>
+    <t>User updated record</t>
+  </si>
+  <si>
     <t>updated_by</t>
   </si>
   <si>
+    <t>Timestamp of record update</t>
+  </si>
+  <si>
     <t>updated_at</t>
   </si>
   <si>
@@ -85,6 +112,9 @@
     <t>Ledger Group</t>
   </si>
   <si>
+    <t>Ledger Group Id</t>
+  </si>
+  <si>
     <t>varchar(2), PK, NN</t>
   </si>
   <si>
@@ -98,6 +128,9 @@
   </si>
   <si>
     <t>ledger_id</t>
+  </si>
+  <si>
+    <t>Representative ledger indicator</t>
   </si>
   <si>
     <t>representative</t>
@@ -145,7 +178,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -191,7 +224,7 @@
         <v>3</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -199,28 +232,28 @@
         <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -228,87 +261,116 @@
         <v>5</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s" s="0">
+      <c r="C5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="G4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="J5" s="0">
-        <f><![CDATA["INSERT INTO """&A$1&"""."""&B$1&""" ("&S5&") VALUES ("&AB5&");" ]]></f>
-      </c>
-      <c r="K5">
-        <f>IF(A5&lt;&gt;"",""""&amp;A$3&amp;"""","")</f>
-      </c>
-      <c r="L5">
-        <f><![CDATA[  K5&IF(AND(K5<>"",B5<>""),", ","")&IF(B5<>"",""""&B$3&"""","") ]]></f>
-      </c>
-      <c r="M5">
-        <f><![CDATA[  L5&IF(AND(L5<>"",C5<>""),", ","")&IF(C5<>"",""""&C$3&"""","") ]]></f>
-      </c>
-      <c r="N5">
-        <f><![CDATA[  M5&IF(AND(M5<>"",D5<>""),", ","")&IF(D5<>"",""""&D$3&"""","") ]]></f>
-      </c>
-      <c r="O5">
-        <f><![CDATA[  N5&IF(AND(N5<>"",E5<>""),", ","")&IF(E5<>"",""""&E$3&"""","") ]]></f>
-      </c>
-      <c r="P5">
-        <f><![CDATA[  O5&IF(AND(O5<>"",F5<>""),", ","")&IF(F5<>"",""""&F$3&"""","") ]]></f>
-      </c>
-      <c r="Q5">
-        <f><![CDATA[  P5&IF(AND(P5<>"",G5<>""),", ","")&IF(G5<>"",""""&G$3&"""","") ]]></f>
-      </c>
-      <c r="R5">
-        <f><![CDATA[  Q5&IF(AND(Q5<>"",H5<>""),", ","")&IF(H5<>"",""""&H$3&"""","") ]]></f>
-      </c>
-      <c r="S5">
-        <f><![CDATA[  R5&IF(AND(R5<>"",I5<>""),", ","")&IF(I5<>"",""""&I$3&"""","") ]]></f>
-      </c>
-      <c r="T5">
-        <f>IF(A5&lt;&gt;"", "'"&amp;A5&amp;"'" ,"")</f>
-      </c>
-      <c r="U5">
-        <f><![CDATA[  T5&IF(AND(T5<>"",B5<>""),", ","")&IF(B5<>"", "'"&B5&"'" ,"") ]]></f>
-      </c>
-      <c r="V5">
-        <f>  U5&amp;IF(AND(U5&lt;&gt;"",C5&lt;&gt;""),", ","")&amp;IF(C5&lt;&gt;"",C5,"") </f>
-      </c>
-      <c r="W5">
-        <f><![CDATA[  V5&IF(AND(V5<>"",D5<>""),", ","")&IF(D5<>"", "'"&D5&"'" ,"") ]]></f>
-      </c>
-      <c r="X5">
-        <f><![CDATA[  W5&IF(AND(W5<>"",E5<>""),", ","")&IF(E5<>"", "'"&E5&"'" ,"") ]]></f>
-      </c>
-      <c r="Y5">
-        <f><![CDATA[  X5&IF(AND(X5<>"",F5<>""),", ","")&IF(F5<>"", "'"&F5&"'" ,"") ]]></f>
-      </c>
-      <c r="Z5">
-        <f><![CDATA[  Y5&IF(AND(Y5<>"",G5<>""),", ","")&IF(G5<>"", "'"&TEXT(G5,"YYYY-MM-DD")&" "&TEXT(G5,"HH:mm:ss")&"'" ,"") ]]></f>
-      </c>
-      <c r="AA5">
-        <f><![CDATA[  Z5&IF(AND(Z5<>"",H5<>""),", ","")&IF(H5<>"", "'"&H5&"'" ,"") ]]></f>
-      </c>
-      <c r="AB5">
-        <f><![CDATA[  AA5&IF(AND(AA5<>"",I5<>""),", ","")&IF(I5<>"", "'"&TEXT(I5,"YYYY-MM-DD")&" "&TEXT(I5,"HH:mm:ss")&"'" ,"") ]]></f>
+      <c r="E5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="J6" s="0">
+        <f><![CDATA["INSERT INTO """&A$1&"""."""&B$1&""" ("&S6&") VALUES ("&AB6&");" ]]></f>
+      </c>
+      <c r="K6">
+        <f>IF(A6&lt;&gt;"",""""&amp;A$4&amp;"""","")</f>
+      </c>
+      <c r="L6">
+        <f><![CDATA[  K6&IF(AND(K6<>"",B6<>""),", ","")&IF(B6<>"",""""&B$4&"""","") ]]></f>
+      </c>
+      <c r="M6">
+        <f><![CDATA[  L6&IF(AND(L6<>"",C6<>""),", ","")&IF(C6<>"",""""&C$4&"""","") ]]></f>
+      </c>
+      <c r="N6">
+        <f><![CDATA[  M6&IF(AND(M6<>"",D6<>""),", ","")&IF(D6<>"",""""&D$4&"""","") ]]></f>
+      </c>
+      <c r="O6">
+        <f><![CDATA[  N6&IF(AND(N6<>"",E6<>""),", ","")&IF(E6<>"",""""&E$4&"""","") ]]></f>
+      </c>
+      <c r="P6">
+        <f><![CDATA[  O6&IF(AND(O6<>"",F6<>""),", ","")&IF(F6<>"",""""&F$4&"""","") ]]></f>
+      </c>
+      <c r="Q6">
+        <f><![CDATA[  P6&IF(AND(P6<>"",G6<>""),", ","")&IF(G6<>"",""""&G$4&"""","") ]]></f>
+      </c>
+      <c r="R6">
+        <f><![CDATA[  Q6&IF(AND(Q6<>"",H6<>""),", ","")&IF(H6<>"",""""&H$4&"""","") ]]></f>
+      </c>
+      <c r="S6">
+        <f><![CDATA[  R6&IF(AND(R6<>"",I6<>""),", ","")&IF(I6<>"",""""&I$4&"""","") ]]></f>
+      </c>
+      <c r="T6">
+        <f>IF(A6&lt;&gt;"", "'"&amp;A6&amp;"'" ,"")</f>
+      </c>
+      <c r="U6">
+        <f><![CDATA[  T6&IF(AND(T6<>"",B6<>""),", ","")&IF(B6<>"", "'"&B6&"'" ,"") ]]></f>
+      </c>
+      <c r="V6">
+        <f>  U6&amp;IF(AND(U6&lt;&gt;"",C6&lt;&gt;""),", ","")&amp;IF(C6&lt;&gt;"",C6,"") </f>
+      </c>
+      <c r="W6">
+        <f><![CDATA[  V6&IF(AND(V6<>"",D6<>""),", ","")&IF(D6<>"", "'"&D6&"'" ,"") ]]></f>
+      </c>
+      <c r="X6">
+        <f><![CDATA[  W6&IF(AND(W6<>"",E6<>""),", ","")&IF(E6<>"", "'"&E6&"'" ,"") ]]></f>
+      </c>
+      <c r="Y6">
+        <f><![CDATA[  X6&IF(AND(X6<>"",F6<>""),", ","")&IF(F6<>"", "'"&F6&"'" ,"") ]]></f>
+      </c>
+      <c r="Z6">
+        <f><![CDATA[  Y6&IF(AND(Y6<>"",G6<>""),", ","")&IF(G6<>"", "'"&TEXT(G6,"YYYY-MM-DD")&" "&TEXT(G6,"HH:mm:ss")&"'" ,"") ]]></f>
+      </c>
+      <c r="AA6">
+        <f><![CDATA[  Z6&IF(AND(Z6<>"",H6<>""),", ","")&IF(H6<>"", "'"&H6&"'" ,"") ]]></f>
+      </c>
+      <c r="AB6">
+        <f><![CDATA[  AA6&IF(AND(AA6<>"",I6<>""),", ","")&IF(I6<>"", "'"&TEXT(I6,"YYYY-MM-DD")&" "&TEXT(I6,"HH:mm:ss")&"'" ,"") ]]></f>
       </c>
     </row>
   </sheetData>
@@ -318,7 +380,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -329,10 +391,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -355,88 +417,108 @@
         <v>3</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>17</v>
-      </c>
       <c r="E4" t="s" s="0">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
-      <c r="G5" s="0">
-        <f><![CDATA["INSERT INTO """&A$1&"""."""&B$1&""" ("&M5&") VALUES ("&S5&");" ]]></f>
-      </c>
-      <c r="H5">
-        <f>IF(A5&lt;&gt;"",""""&amp;A$3&amp;"""","")</f>
-      </c>
-      <c r="I5">
-        <f><![CDATA[  H5&IF(AND(H5<>"",B5<>""),", ","")&IF(B5<>"",""""&B$3&"""","") ]]></f>
-      </c>
-      <c r="J5">
-        <f><![CDATA[  I5&IF(AND(I5<>"",C5<>""),", ","")&IF(C5<>"",""""&C$3&"""","") ]]></f>
-      </c>
-      <c r="K5">
-        <f><![CDATA[  J5&IF(AND(J5<>"",D5<>""),", ","")&IF(D5<>"",""""&D$3&"""","") ]]></f>
-      </c>
-      <c r="L5">
-        <f><![CDATA[  K5&IF(AND(K5<>"",E5<>""),", ","")&IF(E5<>"",""""&E$3&"""","") ]]></f>
-      </c>
-      <c r="M5">
-        <f><![CDATA[  L5&IF(AND(L5<>"",F5<>""),", ","")&IF(F5<>"",""""&F$3&"""","") ]]></f>
-      </c>
-      <c r="N5">
-        <f>IF(A5&lt;&gt;"", "'"&amp;A5&amp;"'" ,"")</f>
-      </c>
-      <c r="O5">
-        <f><![CDATA[  N5&IF(AND(N5<>"",B5<>""),", ","")&IF(B5<>"", "'"&B5&"'" ,"") ]]></f>
-      </c>
-      <c r="P5">
-        <f><![CDATA[  O5&IF(AND(O5<>"",C5<>""),", ","")&IF(C5<>"", "'"&C5&"'" ,"") ]]></f>
-      </c>
-      <c r="Q5">
-        <f><![CDATA[  P5&IF(AND(P5<>"",D5<>""),", ","")&IF(D5<>"", "'"&TEXT(D5,"YYYY-MM-DD")&" "&TEXT(D5,"HH:mm:ss")&"'" ,"") ]]></f>
-      </c>
-      <c r="R5">
-        <f><![CDATA[  Q5&IF(AND(Q5<>"",E5<>""),", ","")&IF(E5<>"", "'"&E5&"'" ,"") ]]></f>
-      </c>
-      <c r="S5">
-        <f><![CDATA[  R5&IF(AND(R5<>"",F5<>""),", ","")&IF(F5<>"", "'"&TEXT(F5,"YYYY-MM-DD")&" "&TEXT(F5,"HH:mm:ss")&"'" ,"") ]]></f>
+      <c r="A5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="G6" s="0">
+        <f><![CDATA["INSERT INTO """&A$1&"""."""&B$1&""" ("&M6&") VALUES ("&S6&");" ]]></f>
+      </c>
+      <c r="H6">
+        <f>IF(A6&lt;&gt;"",""""&amp;A$4&amp;"""","")</f>
+      </c>
+      <c r="I6">
+        <f><![CDATA[  H6&IF(AND(H6<>"",B6<>""),", ","")&IF(B6<>"",""""&B$4&"""","") ]]></f>
+      </c>
+      <c r="J6">
+        <f><![CDATA[  I6&IF(AND(I6<>"",C6<>""),", ","")&IF(C6<>"",""""&C$4&"""","") ]]></f>
+      </c>
+      <c r="K6">
+        <f><![CDATA[  J6&IF(AND(J6<>"",D6<>""),", ","")&IF(D6<>"",""""&D$4&"""","") ]]></f>
+      </c>
+      <c r="L6">
+        <f><![CDATA[  K6&IF(AND(K6<>"",E6<>""),", ","")&IF(E6<>"",""""&E$4&"""","") ]]></f>
+      </c>
+      <c r="M6">
+        <f><![CDATA[  L6&IF(AND(L6<>"",F6<>""),", ","")&IF(F6<>"",""""&F$4&"""","") ]]></f>
+      </c>
+      <c r="N6">
+        <f>IF(A6&lt;&gt;"", "'"&amp;A6&amp;"'" ,"")</f>
+      </c>
+      <c r="O6">
+        <f><![CDATA[  N6&IF(AND(N6<>"",B6<>""),", ","")&IF(B6<>"", "'"&B6&"'" ,"") ]]></f>
+      </c>
+      <c r="P6">
+        <f><![CDATA[  O6&IF(AND(O6<>"",C6<>""),", ","")&IF(C6<>"", "'"&C6&"'" ,"") ]]></f>
+      </c>
+      <c r="Q6">
+        <f><![CDATA[  P6&IF(AND(P6<>"",D6<>""),", ","")&IF(D6<>"", "'"&TEXT(D6,"YYYY-MM-DD")&" "&TEXT(D6,"HH:mm:ss")&"'" ,"") ]]></f>
+      </c>
+      <c r="R6">
+        <f><![CDATA[  Q6&IF(AND(Q6<>"",E6<>""),", ","")&IF(E6<>"", "'"&E6&"'" ,"") ]]></f>
+      </c>
+      <c r="S6">
+        <f><![CDATA[  R6&IF(AND(R6<>"",F6<>""),", ","")&IF(F6<>"", "'"&TEXT(F6,"YYYY-MM-DD")&" "&TEXT(F6,"HH:mm:ss")&"'" ,"") ]]></f>
       </c>
     </row>
   </sheetData>
@@ -446,7 +528,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -457,10 +539,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
@@ -486,100 +568,123 @@
         <v>3</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>27</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>17</v>
-      </c>
       <c r="F4" t="s" s="0">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
-      <c r="H5" s="0">
-        <f><![CDATA["INSERT INTO """&A$1&"""."""&B$1&""" ("&O5&") VALUES ("&V5&");" ]]></f>
-      </c>
-      <c r="I5">
-        <f>IF(A5&lt;&gt;"",""""&amp;A$3&amp;"""","")</f>
-      </c>
-      <c r="J5">
-        <f><![CDATA[  I5&IF(AND(I5<>"",B5<>""),", ","")&IF(B5<>"",""""&B$3&"""","") ]]></f>
-      </c>
-      <c r="K5">
-        <f><![CDATA[  J5&IF(AND(J5<>"",C5<>""),", ","")&IF(C5<>"",""""&C$3&"""","") ]]></f>
-      </c>
-      <c r="L5">
-        <f><![CDATA[  K5&IF(AND(K5<>"",D5<>""),", ","")&IF(D5<>"",""""&D$3&"""","") ]]></f>
-      </c>
-      <c r="M5">
-        <f><![CDATA[  L5&IF(AND(L5<>"",E5<>""),", ","")&IF(E5<>"",""""&E$3&"""","") ]]></f>
-      </c>
-      <c r="N5">
-        <f><![CDATA[  M5&IF(AND(M5<>"",F5<>""),", ","")&IF(F5<>"",""""&F$3&"""","") ]]></f>
-      </c>
-      <c r="O5">
-        <f><![CDATA[  N5&IF(AND(N5<>"",G5<>""),", ","")&IF(G5<>"",""""&G$3&"""","") ]]></f>
-      </c>
-      <c r="P5">
-        <f>IF(A5&lt;&gt;"", "'"&amp;A5&amp;"'" ,"")</f>
-      </c>
-      <c r="Q5">
-        <f><![CDATA[  P5&IF(AND(P5<>"",B5<>""),", ","")&IF(B5<>"", "'"&B5&"'" ,"") ]]></f>
-      </c>
-      <c r="R5">
-        <f>  Q5&amp;IF(AND(Q5&lt;&gt;"",C5&lt;&gt;""),", ","")&amp;IF(C5&lt;&gt;"",C5,"") </f>
-      </c>
-      <c r="S5">
-        <f><![CDATA[  R5&IF(AND(R5<>"",D5<>""),", ","")&IF(D5<>"", "'"&D5&"'" ,"") ]]></f>
-      </c>
-      <c r="T5">
-        <f><![CDATA[  S5&IF(AND(S5<>"",E5<>""),", ","")&IF(E5<>"", "'"&TEXT(E5,"YYYY-MM-DD")&" "&TEXT(E5,"HH:mm:ss")&"'" ,"") ]]></f>
-      </c>
-      <c r="U5">
-        <f><![CDATA[  T5&IF(AND(T5<>"",F5<>""),", ","")&IF(F5<>"", "'"&F5&"'" ,"") ]]></f>
-      </c>
-      <c r="V5">
-        <f><![CDATA[  U5&IF(AND(U5<>"",G5<>""),", ","")&IF(G5<>"", "'"&TEXT(G5,"YYYY-MM-DD")&" "&TEXT(G5,"HH:mm:ss")&"'" ,"") ]]></f>
+      <c r="A5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="H6" s="0">
+        <f><![CDATA["INSERT INTO """&A$1&"""."""&B$1&""" ("&O6&") VALUES ("&V6&");" ]]></f>
+      </c>
+      <c r="I6">
+        <f>IF(A6&lt;&gt;"",""""&amp;A$4&amp;"""","")</f>
+      </c>
+      <c r="J6">
+        <f><![CDATA[  I6&IF(AND(I6<>"",B6<>""),", ","")&IF(B6<>"",""""&B$4&"""","") ]]></f>
+      </c>
+      <c r="K6">
+        <f><![CDATA[  J6&IF(AND(J6<>"",C6<>""),", ","")&IF(C6<>"",""""&C$4&"""","") ]]></f>
+      </c>
+      <c r="L6">
+        <f><![CDATA[  K6&IF(AND(K6<>"",D6<>""),", ","")&IF(D6<>"",""""&D$4&"""","") ]]></f>
+      </c>
+      <c r="M6">
+        <f><![CDATA[  L6&IF(AND(L6<>"",E6<>""),", ","")&IF(E6<>"",""""&E$4&"""","") ]]></f>
+      </c>
+      <c r="N6">
+        <f><![CDATA[  M6&IF(AND(M6<>"",F6<>""),", ","")&IF(F6<>"",""""&F$4&"""","") ]]></f>
+      </c>
+      <c r="O6">
+        <f><![CDATA[  N6&IF(AND(N6<>"",G6<>""),", ","")&IF(G6<>"",""""&G$4&"""","") ]]></f>
+      </c>
+      <c r="P6">
+        <f>IF(A6&lt;&gt;"", "'"&amp;A6&amp;"'" ,"")</f>
+      </c>
+      <c r="Q6">
+        <f><![CDATA[  P6&IF(AND(P6<>"",B6<>""),", ","")&IF(B6<>"", "'"&B6&"'" ,"") ]]></f>
+      </c>
+      <c r="R6">
+        <f>  Q6&amp;IF(AND(Q6&lt;&gt;"",C6&lt;&gt;""),", ","")&amp;IF(C6&lt;&gt;"",C6,"") </f>
+      </c>
+      <c r="S6">
+        <f><![CDATA[  R6&IF(AND(R6<>"",D6<>""),", ","")&IF(D6<>"", "'"&D6&"'" ,"") ]]></f>
+      </c>
+      <c r="T6">
+        <f><![CDATA[  S6&IF(AND(S6<>"",E6<>""),", ","")&IF(E6<>"", "'"&TEXT(E6,"YYYY-MM-DD")&" "&TEXT(E6,"HH:mm:ss")&"'" ,"") ]]></f>
+      </c>
+      <c r="U6">
+        <f><![CDATA[  T6&IF(AND(T6<>"",F6<>""),", ","")&IF(F6<>"", "'"&F6&"'" ,"") ]]></f>
+      </c>
+      <c r="V6">
+        <f><![CDATA[  U6&IF(AND(U6<>"",G6<>""),", ","")&IF(G6<>"", "'"&TEXT(G6,"YYYY-MM-DD")&" "&TEXT(G6,"HH:mm:ss")&"'" ,"") ]]></f>
       </c>
     </row>
   </sheetData>

</xml_diff>